<commit_message>
Empezando casos de prueba nuevos
Signed-off-by: qa-katalon <qa-katalon@DEV-QA-KatalonStudio.BMinc.eu>
</commit_message>
<xml_diff>
--- a/Data Files/TestData/Balance hace match con informacion en CM (C3777).xlsx
+++ b/Data Files/TestData/Balance hace match con informacion en CM (C3777).xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="60">
   <si>
     <t>URL</t>
   </si>
@@ -195,6 +195,15 @@
   </si>
   <si>
     <t>13:30:52.373</t>
+  </si>
+  <si>
+    <t>16/10/2019</t>
+  </si>
+  <si>
+    <t>09:39:18.263</t>
+  </si>
+  <si>
+    <t>09:40:29.013</t>
   </si>
 </sst>
 </file>
@@ -589,16 +598,16 @@
         <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="G2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="H2" t="s">
         <v>31</v>

</xml_diff>